<commit_message>
lambrechts 6653: use cellranger instead of dropSeqPipe.
</commit_message>
<xml_diff>
--- a/raw/lambrechts_2018_6653/samples.xlsx
+++ b/raw/lambrechts_2018_6653/samples.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\single_cell_data_integration\raw\lambrechts_2018_6653\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD189273-37A6-4288-97DA-B31B72B55A6D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67E420E3-1479-4BB6-8D34-749EA958A616}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="8445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E-MTAB-6653.sdrf" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -676,7 +676,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1510,16 +1510,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>LEFT(AT2,FIND("_",AT2)-1)</f>
+        <f t="shared" ref="A2:A12" si="0">LEFT(AT2,FIND("_S",AT2)-1)</f>
         <v>scrBT1429m</v>
       </c>
       <c r="B2">
@@ -1885,7 +1885,7 @@
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A13" si="0">LEFT(AT3,FIND("_",AT3)-1)</f>
+        <f t="shared" si="0"/>
         <v>scrBT1430m</v>
       </c>
       <c r="B3">
@@ -3125,7 +3125,7 @@
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>scrBT1425</v>
+        <v>scrBT1425_hg19</v>
       </c>
       <c r="B10">
         <v>4000</v>
@@ -3302,7 +3302,7 @@
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>scrBT1426</v>
+        <v>scrBT1426_hg19</v>
       </c>
       <c r="B11">
         <v>4000</v>
@@ -3479,7 +3479,7 @@
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>scrBT1427</v>
+        <v>scrBT1427_hg19</v>
       </c>
       <c r="B12">
         <v>4000</v>
@@ -3655,8 +3655,8 @@
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>scrBT1428</v>
+        <f>LEFT(AT13,FIND("_S",AT13)-1)</f>
+        <v>scrBT1428_hg19</v>
       </c>
       <c r="B13">
         <v>4000</v>

</xml_diff>